<commit_message>
Conexion a la base de datos
Se agregaron los .jar correspondientes al framework de persistencia mybatis, tambien el xml de configuracion y la conexion a la base de datos
</commit_message>
<xml_diff>
--- a/Juan/Reviciones/Plantilla_Lista_de_Tareas_de_la_revisión_2.xlsx
+++ b/Juan/Reviciones/Plantilla_Lista_de_Tareas_de_la_revisión_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juuan\Desktop\6to semstre\Des. Software\Proyecto\EmpenioFacil\Juan\Reviciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD56FB-FCE0-4114-BD8E-9B575D9B13A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28646878-B549-466A-8A66-D59AC66E0F86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="589" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -464,9 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,10 +772,10 @@
   <dimension ref="B1:BA40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AG36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AG6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AL39" sqref="AL39"/>
+      <selection pane="bottomRight" activeCell="AX28" sqref="AX28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,24 +2084,26 @@
         <v>75</v>
       </c>
       <c r="AT14" s="9"/>
-      <c r="AU14" s="7"/>
+      <c r="AU14" s="7">
+        <v>10</v>
+      </c>
       <c r="AV14" s="7">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="AW14" s="9"/>
       <c r="AX14" s="7"/>
       <c r="AY14" s="7">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="AZ14" s="10">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="BA14" s="10">
         <f t="shared" si="15"/>
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -3003,24 +3002,26 @@
         <v>80</v>
       </c>
       <c r="AT22" s="9"/>
-      <c r="AU22" s="7"/>
+      <c r="AU22" s="7">
+        <v>10</v>
+      </c>
       <c r="AV22" s="7">
         <f t="shared" si="12"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AW22" s="9"/>
       <c r="AX22" s="7"/>
       <c r="AY22" s="7">
         <f t="shared" si="13"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AZ22" s="10">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA22" s="10">
         <f t="shared" si="15"/>
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -3032,7 +3033,7 @@
       <c r="E23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="4" t="s">
         <v>78</v>
       </c>
       <c r="G23" s="4">
@@ -3693,24 +3694,26 @@
         <v>120</v>
       </c>
       <c r="AT28" s="9"/>
-      <c r="AU28" s="7"/>
+      <c r="AU28" s="7">
+        <v>10</v>
+      </c>
       <c r="AV28" s="7">
         <f t="shared" si="12"/>
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AW28" s="9"/>
       <c r="AX28" s="7"/>
       <c r="AY28" s="7">
         <f t="shared" si="13"/>
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AZ28" s="10">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA28" s="10">
         <f t="shared" si="17"/>
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -4613,24 +4616,26 @@
         <v>85</v>
       </c>
       <c r="AT36" s="9"/>
-      <c r="AU36" s="7"/>
+      <c r="AU36" s="7">
+        <v>10</v>
+      </c>
       <c r="AV36" s="7">
         <f t="shared" si="12"/>
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AW36" s="9"/>
       <c r="AX36" s="7"/>
       <c r="AY36" s="7">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AZ36" s="10">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="BA36" s="10">
         <f t="shared" si="17"/>
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -5085,11 +5090,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5101,6 +5101,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>